<commit_message>
Tweaks to month names
</commit_message>
<xml_diff>
--- a/plymouth/Plymouth_Pressure_Digitised_1874.xlsx
+++ b/plymouth/Plymouth_Pressure_Digitised_1874.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\research\dpv\uk\dwr_plymouth_1873-9AND1891-1921\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed/Documents/GitHub/weather-rescue/plymouth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFD31E1-E7C7-4BBD-8E07-2192F4EFFD5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E243FCF2-DB5B-0D4A-9569-E40C87564CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{05A01184-34FC-49EB-9EDB-CE168D0F5C49}"/>
+    <workbookView xWindow="820" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{05A01184-34FC-49EB-9EDB-CE168D0F5C49}"/>
   </bookViews>
   <sheets>
     <sheet name="Jan1874" sheetId="23" r:id="rId1"/>
     <sheet name="Feb1874" sheetId="22" r:id="rId2"/>
-    <sheet name="March1874" sheetId="21" r:id="rId3"/>
-    <sheet name="April1874" sheetId="1" r:id="rId4"/>
+    <sheet name="Mar1874" sheetId="21" r:id="rId3"/>
+    <sheet name="Apr1874" sheetId="1" r:id="rId4"/>
     <sheet name="May1874" sheetId="18" r:id="rId5"/>
     <sheet name="June1874" sheetId="13" r:id="rId6"/>
     <sheet name="July1874" sheetId="14" r:id="rId7"/>
@@ -112,19 +112,13 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -174,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -189,12 +183,11 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,9 +212,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -259,7 +252,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -365,7 +358,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -507,7 +500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,47 +530,47 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -597,7 +590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -620,7 +613,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -643,7 +636,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -666,7 +659,7 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -689,7 +682,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -712,7 +705,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -735,7 +728,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -758,7 +751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -781,7 +774,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -804,7 +797,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -827,7 +820,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -850,7 +843,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -873,7 +866,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -896,7 +889,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -919,7 +912,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -942,7 +935,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -965,7 +958,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -988,7 +981,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -1011,7 +1004,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -1034,7 +1027,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -1057,7 +1050,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -1080,7 +1073,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -1103,7 +1096,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -1126,7 +1119,7 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -1149,7 +1142,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -1172,7 +1165,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -1195,7 +1188,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -1218,7 +1211,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -1241,7 +1234,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -1264,7 +1257,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -1287,7 +1280,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -1310,7 +1303,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>
@@ -1335,45 +1328,45 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1393,7 +1386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1416,7 +1409,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1439,7 +1432,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -1462,7 +1455,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -1472,7 +1465,7 @@
       <c r="C7" s="7">
         <v>55</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1483,7 +1476,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -1506,7 +1499,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -1529,7 +1522,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1552,7 +1545,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -1575,7 +1568,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -1598,7 +1591,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -1621,7 +1614,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -1644,7 +1637,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -1667,7 +1660,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -1690,7 +1683,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -1713,7 +1706,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -1736,7 +1729,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -1759,7 +1752,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -1782,7 +1775,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -1805,7 +1798,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -1828,7 +1821,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -1851,7 +1844,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -1874,7 +1867,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -1897,7 +1890,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -1920,7 +1913,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -1943,7 +1936,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -1966,7 +1959,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -1989,7 +1982,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -2012,7 +2005,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -2035,7 +2028,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -2058,7 +2051,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -2081,7 +2074,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -2104,7 +2097,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>
@@ -2125,49 +2118,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE413E1-0D8A-47A5-AC42-A5D94E8AF531}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2187,7 +2180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -2210,7 +2203,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -2233,7 +2226,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -2256,7 +2249,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -2279,7 +2272,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -2302,7 +2295,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -2325,7 +2318,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -2348,7 +2341,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -2371,7 +2364,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -2394,7 +2387,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -2417,7 +2410,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -2440,7 +2433,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -2463,7 +2456,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -2486,7 +2479,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -2502,14 +2495,14 @@
       <c r="E17" s="7">
         <v>44</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>29.21</v>
       </c>
       <c r="G17" s="7">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -2532,7 +2525,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -2555,7 +2548,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -2578,7 +2571,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -2601,7 +2594,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -2624,7 +2617,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -2647,7 +2640,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -2670,7 +2663,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -2693,7 +2686,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -2716,7 +2709,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -2739,7 +2732,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -2762,7 +2755,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -2785,7 +2778,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -2808,7 +2801,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -2831,7 +2824,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -2854,7 +2847,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -2877,7 +2870,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -2888,7 +2881,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>
@@ -2914,45 +2907,45 @@
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -2972,7 +2965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -2995,7 +2988,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -3018,7 +3011,7 @@
         <v>39.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -3041,7 +3034,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -3064,7 +3057,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -3087,7 +3080,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -3110,7 +3103,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -3133,7 +3126,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -3156,7 +3149,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -3179,7 +3172,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -3202,7 +3195,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -3225,7 +3218,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -3248,7 +3241,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -3271,7 +3264,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -3294,7 +3287,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -3317,7 +3310,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -3340,7 +3333,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -3363,7 +3356,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -3386,7 +3379,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -3409,7 +3402,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -3432,7 +3425,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -3455,7 +3448,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -3478,7 +3471,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -3501,7 +3494,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -3524,7 +3517,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -3547,7 +3540,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -3570,7 +3563,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -3593,7 +3586,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -3616,7 +3609,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -3639,7 +3632,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -3662,7 +3655,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -3685,7 +3678,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>
@@ -3710,46 +3703,46 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -3769,7 +3762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -3792,7 +3785,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -3815,7 +3808,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -3838,7 +3831,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -3861,7 +3854,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -3884,7 +3877,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -3907,7 +3900,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -3930,7 +3923,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -3953,7 +3946,7 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -3976,7 +3969,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -3999,7 +3992,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -4022,7 +4015,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -4045,7 +4038,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -4068,7 +4061,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -4091,7 +4084,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -4114,7 +4107,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -4137,7 +4130,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -4160,7 +4153,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -4183,7 +4176,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -4206,7 +4199,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -4229,7 +4222,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -4252,7 +4245,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -4275,7 +4268,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -4298,7 +4291,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -4321,7 +4314,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -4344,7 +4337,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -4367,7 +4360,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -4390,7 +4383,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -4413,7 +4406,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -4424,7 +4417,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -4435,7 +4428,7 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -4446,7 +4439,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
     </row>
   </sheetData>
@@ -4470,45 +4463,45 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.5" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -4528,7 +4521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -4551,7 +4544,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -4574,7 +4567,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -4597,7 +4590,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -4620,7 +4613,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -4636,14 +4629,12 @@
       <c r="E8" s="7">
         <v>48</v>
       </c>
-      <c r="F8" s="10">
-        <v>30.52</v>
-      </c>
+      <c r="F8" s="6"/>
       <c r="G8" s="7">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -4666,7 +4657,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -4689,7 +4680,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -4712,7 +4703,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -4735,7 +4726,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -4758,7 +4749,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -4781,7 +4772,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -4804,7 +4795,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -4827,7 +4818,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -4850,7 +4841,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -4873,7 +4864,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -4896,7 +4887,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -4919,7 +4910,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -4942,7 +4933,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="6">
         <v>30.154</v>
@@ -4963,7 +4954,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -4986,7 +4977,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -5009,7 +5000,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -5032,7 +5023,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -5055,7 +5046,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -5078,7 +5069,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -5101,7 +5092,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -5124,7 +5115,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -5147,7 +5138,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -5170,7 +5161,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -5193,7 +5184,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -5216,7 +5207,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -5239,7 +5230,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>
@@ -5264,45 +5255,45 @@
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -5322,7 +5313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -5345,7 +5336,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -5368,7 +5359,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -5391,7 +5382,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -5414,7 +5405,7 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -5437,7 +5428,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -5460,7 +5451,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -5483,7 +5474,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -5506,7 +5497,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -5529,7 +5520,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -5552,7 +5543,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -5575,7 +5566,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -5598,7 +5589,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -5621,7 +5612,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -5644,7 +5635,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -5667,7 +5658,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -5690,7 +5681,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -5713,7 +5704,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -5736,7 +5727,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -5759,7 +5750,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -5782,7 +5773,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -5805,7 +5796,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -5828,7 +5819,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -5851,7 +5842,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -5874,7 +5865,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -5897,7 +5888,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -5920,7 +5911,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -5943,7 +5934,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -5966,7 +5957,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -5989,7 +5980,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -6012,7 +6003,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -6023,7 +6014,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>
@@ -6044,50 +6035,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CFA230-87CD-458D-AE20-523033105AC7}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView zoomScale="98" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -6107,7 +6098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -6130,7 +6121,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -6153,7 +6144,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -6176,7 +6167,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -6199,7 +6190,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -6222,7 +6213,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -6245,7 +6236,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -6268,7 +6259,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -6291,7 +6282,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -6314,7 +6305,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -6337,7 +6328,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -6360,7 +6351,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -6383,7 +6374,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -6406,7 +6397,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -6429,7 +6420,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -6452,7 +6443,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -6475,7 +6466,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -6498,7 +6489,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -6521,7 +6512,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -6544,7 +6535,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -6567,7 +6558,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -6590,7 +6581,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -6613,7 +6604,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -6636,7 +6627,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -6659,7 +6650,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -6682,7 +6673,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -6705,7 +6696,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -6728,7 +6719,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -6751,7 +6742,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -6774,7 +6765,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -6797,7 +6788,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -6820,7 +6811,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>
@@ -6845,45 +6836,45 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -6903,7 +6894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -6926,7 +6917,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -6949,7 +6940,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -6972,7 +6963,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -6995,7 +6986,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -7018,7 +7009,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -7041,7 +7032,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -7064,7 +7055,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -7087,7 +7078,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -7110,7 +7101,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -7133,7 +7124,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -7156,7 +7147,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -7179,7 +7170,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -7202,7 +7193,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -7225,7 +7216,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -7248,7 +7239,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -7271,7 +7262,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -7294,7 +7285,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -7317,7 +7308,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -7340,7 +7331,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -7363,7 +7354,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -7386,7 +7377,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -7409,7 +7400,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -7432,7 +7423,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -7455,7 +7446,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -7478,7 +7469,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -7501,7 +7492,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -7524,7 +7515,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -7547,7 +7538,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -7570,7 +7561,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -7593,7 +7584,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -7604,7 +7595,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>
@@ -7629,45 +7620,45 @@
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -7687,7 +7678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -7710,7 +7701,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -7733,7 +7724,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -7756,7 +7747,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -7779,7 +7770,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -7802,7 +7793,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -7825,7 +7816,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -7848,7 +7839,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -7871,7 +7862,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -7894,7 +7885,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -7917,7 +7908,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -7940,7 +7931,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -7963,7 +7954,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -7986,7 +7977,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -8009,7 +8000,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -8032,7 +8023,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -8055,7 +8046,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -8078,7 +8069,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -8101,7 +8092,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -8124,7 +8115,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -8147,7 +8138,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -8170,7 +8161,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -8193,7 +8184,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -8216,7 +8207,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -8239,7 +8230,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -8262,7 +8253,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -8285,7 +8276,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -8308,7 +8299,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -8331,7 +8322,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -8354,7 +8345,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -8377,7 +8368,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -8400,7 +8391,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>
@@ -8425,45 +8416,45 @@
       <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -8483,7 +8474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -8506,7 +8497,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -8529,7 +8520,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -8552,7 +8543,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -8575,7 +8566,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -8598,7 +8589,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -8621,7 +8612,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -8644,7 +8635,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -8667,7 +8658,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -8690,7 +8681,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -8713,7 +8704,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -8736,7 +8727,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -8759,7 +8750,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -8782,7 +8773,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -8805,7 +8796,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -8828,7 +8819,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -8851,7 +8842,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -8874,7 +8865,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -8897,7 +8888,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -8920,7 +8911,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -8943,7 +8934,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -8966,7 +8957,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -8989,7 +8980,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -9012,7 +9003,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -9035,7 +9026,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -9058,7 +9049,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -9081,7 +9072,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -9104,7 +9095,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -9127,7 +9118,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -9150,7 +9141,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -9173,7 +9164,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -9196,7 +9187,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>
@@ -9221,45 +9212,45 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -9279,7 +9270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -9302,7 +9293,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -9325,7 +9316,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -9335,7 +9326,7 @@
       <c r="C6" s="7">
         <v>62</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>29.600999999999999</v>
       </c>
       <c r="E6" s="7">
@@ -9348,7 +9339,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -9371,7 +9362,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -9394,7 +9385,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -9417,7 +9408,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -9440,7 +9431,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -9463,7 +9454,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -9486,7 +9477,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -9509,7 +9500,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -9532,7 +9523,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -9555,7 +9546,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -9578,7 +9569,7 @@
         <v>59.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -9601,7 +9592,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -9624,7 +9615,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -9647,7 +9638,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -9670,7 +9661,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -9693,7 +9684,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -9716,7 +9707,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -9739,7 +9730,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -9762,7 +9753,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -9785,7 +9776,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -9808,7 +9799,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -9831,7 +9822,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -9854,7 +9845,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -9877,7 +9868,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -9900,7 +9891,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -9923,7 +9914,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -9946,7 +9937,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -9969,7 +9960,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -9980,7 +9971,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="D35" s="1"/>
     </row>

</xml_diff>